<commit_message>
write result of questionnaire
</commit_message>
<xml_diff>
--- a/literature/04.reseach-interface-comparative-experiments/アンケート　結果.xlsx
+++ b/literature/04.reseach-interface-comparative-experiments/アンケート　結果.xlsx
@@ -16,7 +16,6 @@
     <sheet name="相関ごと分析" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="78">
   <si>
     <t>操作のわかりやすさ</t>
   </si>
@@ -432,6 +431,10 @@
     <t>グラフあり</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>見やすさ</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -1165,6 +1168,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,12 +1181,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1676,11 +1679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122838024"/>
-        <c:axId val="-2122835048"/>
+        <c:axId val="-2127345224"/>
+        <c:axId val="-2121923528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122838024"/>
+        <c:axId val="-2127345224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,7 +1693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122835048"/>
+        <c:crossAx val="-2121923528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1698,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122835048"/>
+        <c:axId val="-2121923528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -1729,7 +1732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122838024"/>
+        <c:crossAx val="-2127345224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1877,11 +1880,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128354104"/>
-        <c:axId val="-2126918072"/>
+        <c:axId val="2121517640"/>
+        <c:axId val="2121513640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128354104"/>
+        <c:axId val="2121517640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1893,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126918072"/>
+        <c:crossAx val="2121513640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1898,7 +1901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126918072"/>
+        <c:axId val="2121513640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0"/>
@@ -1928,7 +1931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128354104"/>
+        <c:crossAx val="2121517640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2027,11 +2030,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2126808168"/>
-        <c:axId val="-2128590536"/>
+        <c:axId val="-2125133736"/>
+        <c:axId val="-2122657160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126808168"/>
+        <c:axId val="-2125133736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2043,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128590536"/>
+        <c:crossAx val="-2122657160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2048,7 +2051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128590536"/>
+        <c:axId val="-2122657160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2059,7 +2062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126808168"/>
+        <c:crossAx val="-2125133736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2188,11 +2191,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125109944"/>
-        <c:axId val="-2129832536"/>
+        <c:axId val="2120664120"/>
+        <c:axId val="-2128386840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125109944"/>
+        <c:axId val="2120664120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +2205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129832536"/>
+        <c:crossAx val="-2128386840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2210,7 +2213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129832536"/>
+        <c:axId val="-2128386840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -2241,7 +2244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125109944"/>
+        <c:crossAx val="2120664120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2386,11 +2389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122614024"/>
-        <c:axId val="-2130455704"/>
+        <c:axId val="-2128335832"/>
+        <c:axId val="-2127230632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122614024"/>
+        <c:axId val="-2128335832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130455704"/>
+        <c:crossAx val="-2127230632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2408,7 +2411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130455704"/>
+        <c:axId val="-2127230632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,7 +2422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122614024"/>
+        <c:crossAx val="-2128335832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2548,11 +2551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125410280"/>
-        <c:axId val="-2130546760"/>
+        <c:axId val="-2126895208"/>
+        <c:axId val="-2128454792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125410280"/>
+        <c:axId val="-2126895208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2562,7 +2565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130546760"/>
+        <c:crossAx val="-2128454792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2570,7 +2573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130546760"/>
+        <c:axId val="-2128454792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -2601,7 +2604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125410280"/>
+        <c:crossAx val="-2126895208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2746,11 +2749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2123233480"/>
-        <c:axId val="-2124737064"/>
+        <c:axId val="-2126170776"/>
+        <c:axId val="-2124787832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2123233480"/>
+        <c:axId val="-2126170776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2760,7 +2763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124737064"/>
+        <c:crossAx val="-2124787832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2768,7 +2771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124737064"/>
+        <c:axId val="-2124787832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123233480"/>
+        <c:crossAx val="-2126170776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3048,11 +3051,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124921208"/>
-        <c:axId val="-2123165320"/>
+        <c:axId val="2038469400"/>
+        <c:axId val="-2123461224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124921208"/>
+        <c:axId val="2038469400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3072,7 +3075,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123165320"/>
+        <c:crossAx val="-2123461224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3080,7 +3083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123165320"/>
+        <c:axId val="-2123461224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0"/>
@@ -3112,7 +3115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124921208"/>
+        <c:crossAx val="2038469400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3238,7 +3241,7 @@
                   <c:v>構成のわかりやすさ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>見易さ</c:v>
+                  <c:v>見やすさ</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>反応のよさ</c:v>
@@ -3351,7 +3354,7 @@
                   <c:v>構成のわかりやすさ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>見易さ</c:v>
+                  <c:v>見やすさ</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>反応のよさ</c:v>
@@ -3390,11 +3393,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2126066648"/>
-        <c:axId val="2119532040"/>
+        <c:axId val="-2125750552"/>
+        <c:axId val="-2130694696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126066648"/>
+        <c:axId val="-2125750552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,7 +3416,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119532040"/>
+        <c:crossAx val="-2130694696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3421,7 +3424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119532040"/>
+        <c:axId val="-2130694696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3456,12 +3459,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100"/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126066648"/>
+        <c:crossAx val="-2125750552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3485,6 +3488,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3788,11 +3796,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2126595288"/>
-        <c:axId val="2084054056"/>
+        <c:axId val="-2123774920"/>
+        <c:axId val="2101779992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126595288"/>
+        <c:axId val="-2123774920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3801,7 +3809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084054056"/>
+        <c:crossAx val="2101779992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3809,7 +3817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2084054056"/>
+        <c:axId val="2101779992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3819,7 +3827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126595288"/>
+        <c:crossAx val="-2123774920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3971,11 +3979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128576136"/>
-        <c:axId val="-2126623544"/>
+        <c:axId val="2121859928"/>
+        <c:axId val="2121569192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128576136"/>
+        <c:axId val="2121859928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3985,7 +3993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126623544"/>
+        <c:crossAx val="2121569192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3993,7 +4001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126623544"/>
+        <c:axId val="2121569192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4022,7 +4030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128576136"/>
+        <c:crossAx val="2121859928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6129,13 +6137,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="D16:D18"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="H8:H10"/>
@@ -6145,6 +6146,13 @@
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="G11:G13"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="D16:D18"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6162,8 +6170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -6183,17 +6191,17 @@
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="51">
         <v>4.4444444444444455</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="50">
         <v>3.8888888888888893</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="41"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="53"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="50"/>
       <c r="E4" s="36">
         <v>4.4444444444444455</v>
       </c>
@@ -6203,8 +6211,8 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="41"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="50"/>
       <c r="E5" s="36">
         <v>4.333333333333333</v>
       </c>
@@ -6216,10 +6224,10 @@
       <c r="A6" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="51">
         <v>4.333333333333333</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="50">
         <v>4.4444444444444438</v>
       </c>
       <c r="E6" s="36">
@@ -6231,8 +6239,8 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="42"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="50"/>
       <c r="E7" s="36">
         <v>4.2222222222222223</v>
       </c>
@@ -6242,8 +6250,8 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="42"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="50"/>
       <c r="E8" s="36"/>
       <c r="F8" s="37"/>
     </row>
@@ -6251,10 +6259,10 @@
       <c r="A9" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="51">
         <v>4.4444444444444438</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="50">
         <v>4.5555555555555545</v>
       </c>
       <c r="E9" s="36"/>
@@ -6262,13 +6270,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="43"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="43"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="53"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="50"/>
       <c r="E11" s="36"/>
       <c r="F11" s="37"/>
     </row>
@@ -6276,10 +6284,10 @@
       <c r="A12" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="51">
         <v>4.2222222222222223</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="50">
         <v>4.5555555555555554</v>
       </c>
       <c r="E12" s="36"/>
@@ -6287,13 +6295,13 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="44"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="50"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="44"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="53"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="50"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
     </row>
@@ -6335,7 +6343,7 @@
       <c r="D20" s="49">
         <v>3.8888888888888893</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="52">
         <v>0.8388704928078603</v>
       </c>
     </row>
@@ -6343,13 +6351,13 @@
       <c r="B21" s="49"/>
       <c r="C21" s="35"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="51"/>
+      <c r="E21" s="53"/>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="49"/>
       <c r="C22" s="35"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="52"/>
+      <c r="E22" s="54"/>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" s="49">
@@ -6361,7 +6369,7 @@
       <c r="D23" s="49">
         <v>4.4444444444444438</v>
       </c>
-      <c r="E23" s="50">
+      <c r="E23" s="52">
         <v>0.50917507721731559</v>
       </c>
     </row>
@@ -6369,13 +6377,13 @@
       <c r="B24" s="49"/>
       <c r="C24" s="35"/>
       <c r="D24" s="49"/>
-      <c r="E24" s="51"/>
+      <c r="E24" s="53"/>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="49"/>
       <c r="C25" s="35"/>
       <c r="D25" s="49"/>
-      <c r="E25" s="52"/>
+      <c r="E25" s="54"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="49">
@@ -6387,7 +6395,7 @@
       <c r="D26" s="49">
         <v>4.5555555555555545</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="52">
         <v>0.38490017945975069</v>
       </c>
     </row>
@@ -6395,13 +6403,13 @@
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
-      <c r="E27" s="51"/>
+      <c r="E27" s="53"/>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" s="49"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
-      <c r="E28" s="52"/>
+      <c r="E28" s="54"/>
       <c r="H28" t="s">
         <v>75</v>
       </c>
@@ -6425,7 +6433,7 @@
       <c r="D29" s="35">
         <v>4.5555555555555554</v>
       </c>
-      <c r="E29" s="50">
+      <c r="E29" s="52">
         <v>0.76980035891950038</v>
       </c>
       <c r="G29" t="s">
@@ -6448,7 +6456,7 @@
       <c r="B30" s="49"/>
       <c r="C30" s="49"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="51"/>
+      <c r="E30" s="53"/>
       <c r="G30" t="s">
         <v>1</v>
       </c>
@@ -6469,9 +6477,9 @@
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
       <c r="D31" s="35"/>
-      <c r="E31" s="52"/>
+      <c r="E31" s="54"/>
       <c r="G31" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="H31" s="36">
         <v>4.4444444444444438</v>
@@ -6542,18 +6550,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="E26:E28"/>
     <mergeCell ref="E29:E31"/>
     <mergeCell ref="E23:E25"/>
@@ -6569,6 +6565,18 @@
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="D26:D28"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8431,21 +8439,21 @@
       <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="51">
         <f>AVERAGE(B19:B21)</f>
         <v>4.4444444444444455</v>
       </c>
       <c r="D19">
         <v>4.5</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="51">
         <f>AVERAGE(D19:D21)</f>
         <v>3.5</v>
       </c>
       <c r="F19" s="33">
         <v>5</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="51">
         <f>AVERAGE(F19:F21)</f>
         <v>4.666666666666667</v>
       </c>
@@ -8485,15 +8493,15 @@
       <c r="B20">
         <v>4.666666666666667</v>
       </c>
-      <c r="C20" s="54"/>
+      <c r="C20" s="51"/>
       <c r="D20">
         <v>2.5</v>
       </c>
-      <c r="E20" s="54"/>
+      <c r="E20" s="51"/>
       <c r="F20" s="33">
         <v>4</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="51"/>
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
@@ -8535,15 +8543,15 @@
       <c r="B21">
         <v>4.666666666666667</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="51"/>
       <c r="D21">
         <v>3.5</v>
       </c>
-      <c r="E21" s="54"/>
+      <c r="E21" s="51"/>
       <c r="F21" s="33">
         <v>5</v>
       </c>
-      <c r="G21" s="54"/>
+      <c r="G21" s="51"/>
       <c r="I21" s="1" t="s">
         <v>2</v>
       </c>
@@ -8583,21 +8591,21 @@
       <c r="B22">
         <v>4.333333333333333</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="51">
         <f>AVERAGE(B22:B24)</f>
         <v>4.333333333333333</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="51">
         <f>AVERAGE(D22:D24)</f>
         <v>4.333333333333333</v>
       </c>
       <c r="F22" s="33">
         <v>4</v>
       </c>
-      <c r="G22" s="54">
+      <c r="G22" s="51">
         <f>AVERAGE(F22:F24)</f>
         <v>4.666666666666667</v>
       </c>
@@ -8630,15 +8638,15 @@
       <c r="B23">
         <v>4.666666666666667</v>
       </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="51"/>
       <c r="D23">
         <v>5</v>
       </c>
-      <c r="E23" s="54"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="33">
         <v>5</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="51"/>
       <c r="R23" s="66" t="s">
         <v>37</v>
       </c>
@@ -8650,15 +8658,15 @@
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="51"/>
       <c r="D24">
         <v>4</v>
       </c>
-      <c r="E24" s="54"/>
+      <c r="E24" s="51"/>
       <c r="F24" s="33">
         <v>5</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="51"/>
       <c r="R24" s="66"/>
       <c r="V24" s="33">
         <v>5</v>
@@ -8668,21 +8676,21 @@
       <c r="B25">
         <v>4.333333333333333</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25" s="51">
         <f>AVERAGE(B25:B27)</f>
         <v>4.4444444444444438</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="51">
         <f>AVERAGE(D25:D27)</f>
         <v>4.333333333333333</v>
       </c>
       <c r="F25" s="33">
         <v>5</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="51">
         <f>AVERAGE(F25:F27)</f>
         <v>5</v>
       </c>
@@ -8695,49 +8703,49 @@
       <c r="B26">
         <v>4.333333333333333</v>
       </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="51"/>
       <c r="D26">
         <v>4</v>
       </c>
-      <c r="E26" s="54"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="33">
         <v>5</v>
       </c>
-      <c r="G26" s="54"/>
+      <c r="G26" s="51"/>
     </row>
     <row r="27" spans="2:26">
       <c r="B27">
         <v>4.666666666666667</v>
       </c>
-      <c r="C27" s="54"/>
+      <c r="C27" s="51"/>
       <c r="D27">
         <v>4</v>
       </c>
-      <c r="E27" s="54"/>
+      <c r="E27" s="51"/>
       <c r="F27" s="33">
         <v>5</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" spans="2:26">
       <c r="B28">
         <v>2.6666666666666665</v>
       </c>
-      <c r="C28" s="54">
+      <c r="C28" s="51">
         <f t="shared" ref="C28:E28" si="3">AVERAGE(B28:B30)</f>
         <v>4.2222222222222223</v>
       </c>
       <c r="D28">
         <v>3.5</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="51">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
       <c r="F28" s="33">
         <v>4</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G28" s="51">
         <f t="shared" ref="G28" si="4">AVERAGE(F28:F30)</f>
         <v>4.666666666666667</v>
       </c>
@@ -8746,29 +8754,29 @@
       <c r="B29">
         <v>5</v>
       </c>
-      <c r="C29" s="54"/>
+      <c r="C29" s="51"/>
       <c r="D29">
         <v>5</v>
       </c>
-      <c r="E29" s="54"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="33">
         <v>5</v>
       </c>
-      <c r="G29" s="54"/>
+      <c r="G29" s="51"/>
     </row>
     <row r="30" spans="2:26">
       <c r="B30">
         <v>5</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="51"/>
       <c r="D30">
         <v>5</v>
       </c>
-      <c r="E30" s="54"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="33">
         <v>5</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="51"/>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
@@ -8785,18 +8793,18 @@
       <c r="B36" s="32">
         <v>4</v>
       </c>
-      <c r="C36" s="51">
+      <c r="C36" s="53">
         <f>AVERAGE(B36:B38)</f>
         <v>3</v>
       </c>
-      <c r="D36" s="54">
+      <c r="D36" s="51">
         <f>STDEV(B36:B38)</f>
         <v>1.7320508075688772</v>
       </c>
       <c r="F36" s="28">
         <v>4</v>
       </c>
-      <c r="G36" s="51">
+      <c r="G36" s="53">
         <f>AVERAGE(F36:F38)</f>
         <v>4.666666666666667</v>
       </c>
@@ -8810,12 +8818,12 @@
       <c r="B37" s="32">
         <v>1</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="54"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="51"/>
       <c r="F37" s="28">
         <v>5</v>
       </c>
-      <c r="G37" s="51"/>
+      <c r="G37" s="53"/>
       <c r="H37" s="61"/>
     </row>
     <row r="38" spans="1:8">
@@ -8823,12 +8831,12 @@
       <c r="B38" s="32">
         <v>4</v>
       </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="54"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="51"/>
       <c r="F38" s="28">
         <v>5</v>
       </c>
-      <c r="G38" s="51"/>
+      <c r="G38" s="53"/>
       <c r="H38" s="61"/>
     </row>
     <row r="39" spans="1:8">
@@ -8838,18 +8846,18 @@
       <c r="B39" s="32">
         <v>5</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="53">
         <f>AVERAGE(B39:B41)</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="D39" s="54">
+      <c r="D39" s="51">
         <f t="shared" ref="D39" si="5">STDEV(B39:B41)</f>
         <v>1.154700538379251</v>
       </c>
       <c r="F39" s="28">
         <v>5</v>
       </c>
-      <c r="G39" s="51">
+      <c r="G39" s="53">
         <f t="shared" ref="G39" si="6">AVERAGE(F39:F41)</f>
         <v>5</v>
       </c>
@@ -8863,12 +8871,12 @@
       <c r="B40" s="32">
         <v>5</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="54"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="51"/>
       <c r="F40" s="28">
         <v>5</v>
       </c>
-      <c r="G40" s="51"/>
+      <c r="G40" s="53"/>
       <c r="H40" s="61"/>
     </row>
     <row r="41" spans="1:8">
@@ -8876,12 +8884,12 @@
       <c r="B41" s="32">
         <v>3</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="54"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="51"/>
       <c r="F41" s="28">
         <v>5</v>
       </c>
-      <c r="G41" s="51"/>
+      <c r="G41" s="53"/>
       <c r="H41" s="61"/>
     </row>
     <row r="42" spans="1:8">
@@ -8891,18 +8899,18 @@
       <c r="B42" s="32">
         <v>5</v>
       </c>
-      <c r="C42" s="51">
+      <c r="C42" s="53">
         <f>AVERAGE(B42:B44)</f>
         <v>4</v>
       </c>
-      <c r="D42" s="54">
+      <c r="D42" s="51">
         <f t="shared" ref="D42" si="8">STDEV(B42:B44)</f>
         <v>1</v>
       </c>
       <c r="F42" s="28">
         <v>3</v>
       </c>
-      <c r="G42" s="51">
+      <c r="G42" s="53">
         <f t="shared" ref="G42" si="9">AVERAGE(F42:F44)</f>
         <v>3.6666666666666665</v>
       </c>
@@ -8916,12 +8924,12 @@
       <c r="B43" s="32">
         <v>4</v>
       </c>
-      <c r="C43" s="51"/>
-      <c r="D43" s="54"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="51"/>
       <c r="F43" s="28">
         <v>3</v>
       </c>
-      <c r="G43" s="51"/>
+      <c r="G43" s="53"/>
       <c r="H43" s="61"/>
     </row>
     <row r="44" spans="1:8">
@@ -8929,12 +8937,12 @@
       <c r="B44" s="32">
         <v>3</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="54"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="51"/>
       <c r="F44" s="28">
         <v>5</v>
       </c>
-      <c r="G44" s="51"/>
+      <c r="G44" s="53"/>
       <c r="H44" s="61"/>
     </row>
     <row r="45" spans="1:8">
@@ -8944,18 +8952,18 @@
       <c r="B45" s="32">
         <v>5</v>
       </c>
-      <c r="C45" s="51">
+      <c r="C45" s="53">
         <f t="shared" ref="C45" si="11">AVERAGE(B45:B47)</f>
         <v>5</v>
       </c>
-      <c r="D45" s="54">
+      <c r="D45" s="51">
         <f t="shared" ref="D45" si="12">STDEV(B45:B47)</f>
         <v>0</v>
       </c>
       <c r="F45" s="28">
         <v>2</v>
       </c>
-      <c r="G45" s="51">
+      <c r="G45" s="53">
         <f t="shared" ref="G45" si="13">AVERAGE(F45:F47)</f>
         <v>4</v>
       </c>
@@ -8969,12 +8977,12 @@
       <c r="B46" s="32">
         <v>5</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="54"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="51"/>
       <c r="F46" s="28">
         <v>5</v>
       </c>
-      <c r="G46" s="51"/>
+      <c r="G46" s="53"/>
       <c r="H46" s="61"/>
     </row>
     <row r="47" spans="1:8">
@@ -8982,12 +8990,12 @@
       <c r="B47" s="32">
         <v>5</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="54"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="51"/>
       <c r="F47" s="28">
         <v>5</v>
       </c>
-      <c r="G47" s="51"/>
+      <c r="G47" s="53"/>
       <c r="H47" s="61"/>
     </row>
     <row r="67" spans="3:4">
@@ -9024,6 +9032,40 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="G45:G47"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
     <mergeCell ref="H42:H44"/>
     <mergeCell ref="H45:H47"/>
     <mergeCell ref="R4:R6"/>
@@ -9037,40 +9079,6 @@
     <mergeCell ref="R23:R25"/>
     <mergeCell ref="H36:H38"/>
     <mergeCell ref="H39:H41"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>